<commit_message>
Development of the xls file with description of the DNS geometry.
</commit_message>
<xml_diff>
--- a/MLZ/DNS/dns_draft.xlsx
+++ b/MLZ/DNS/dns_draft.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14540" tabRatio="500"/>
+    <workbookView xWindow="3300" yWindow="3220" windowWidth="25600" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>pixels_per_tube</t>
   </si>
@@ -38,12 +38,6 @@
     <t>m</t>
   </si>
   <si>
-    <t>tube_width</t>
-  </si>
-  <si>
-    <t>tube_thickness</t>
-  </si>
-  <si>
     <t>tube_pressure</t>
   </si>
   <si>
@@ -81,13 +75,34 @@
   </si>
   <si>
     <t>Bank</t>
+  </si>
+  <si>
+    <t>tube_diameter</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>angular_step</t>
+  </si>
+  <si>
+    <t>degree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,6 +122,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,8 +157,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -472,7 +496,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -484,30 +508,30 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -524,10 +548,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -668,10 +692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -680,67 +704,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>960</v>
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>960</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>300</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
+      <c r="C9" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -759,7 +812,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -768,67 +821,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B4">
-        <v>0.15</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>300</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>